<commit_message>
Atualização e limpeza do código.
Divisão de scripts longos em menores
</commit_message>
<xml_diff>
--- a/data/dataset/ControleAtualizacaoOSC.xlsx
+++ b/data/dataset/ControleAtualizacaoOSC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muril\Dropbox\ActiveProjects\IPEAGeral\data\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Murilo\Dropbox\ActiveProjects\mapa-osc-data-import\data\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB67301-C965-439A-9907-ADEFBE25CEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24D4F775-7D34-4EA9-83C3-BE5B09280B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{8BD6E799-85E8-40F6-90D6-44E49F481F67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8BD6E799-85E8-40F6-90D6-44E49F481F67}"/>
   </bookViews>
   <sheets>
     <sheet name="ControleAtualizacao" sheetId="11" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <definedName name="DadosExternos_3" localSheetId="1" hidden="1">ProcessosAtualizacao!$A$1:$I$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Processo</t>
   </si>
@@ -188,6 +189,12 @@
   </si>
   <si>
     <t>Fechamento Atualização</t>
+  </si>
+  <si>
+    <t>Determinação das áreas de atuação com a CNAE secundária (multiáreas)</t>
+  </si>
+  <si>
+    <t>Extrai localização das OSC</t>
   </si>
 </sst>
 </file>
@@ -231,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -249,14 +256,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -271,108 +272,108 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -436,61 +437,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3B1B7FD2-97A2-421B-B66A-371075D2F6B1}" name="ControleAtualizacao" displayName="ControleAtualizacao" ref="A1:H2" tableType="queryTable" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3B1B7FD2-97A2-421B-B66A-371075D2F6B1}" name="ControleAtualizacao" displayName="ControleAtualizacao" ref="A1:H2" tableType="queryTable" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:H2" xr:uid="{3B1B7FD2-97A2-421B-B66A-371075D2F6B1}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B3DD9E4F-9BE2-40BD-A4D3-80045CC727A1}" uniqueName="1" name="At_id" queryTableFieldId="1" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{23B320EC-911E-46EB-BAE9-B25E8B4437ED}" uniqueName="2" name="At_CodRef" queryTableFieldId="2" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{5B2F0353-95F8-4DCF-B3BC-0BBE000EB8F6}" uniqueName="3" name="At_Situacao" queryTableFieldId="3" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E7CE68CB-A1FF-46BC-93BE-9116EBA50B9F}" uniqueName="4" name="At_DataRef" queryTableFieldId="4" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{5C9C4225-6BE7-4955-A793-8C860651F33E}" uniqueName="5" name="At_DataInicio" queryTableFieldId="5" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{893E6C04-AFB9-4B12-A199-D4BE6562C55D}" uniqueName="6" name="At_DataFim" queryTableFieldId="6" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{05DB2C07-4238-48EB-9DF6-4A14F78EB259}" uniqueName="7" name="At_ValidadeDias" queryTableFieldId="7" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{32D990E8-9596-4F1C-801B-85A44CDE7A5D}" uniqueName="8" name="At_DtFimValidade" queryTableFieldId="8" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{B3DD9E4F-9BE2-40BD-A4D3-80045CC727A1}" uniqueName="1" name="At_id" queryTableFieldId="1" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{23B320EC-911E-46EB-BAE9-B25E8B4437ED}" uniqueName="2" name="At_CodRef" queryTableFieldId="2" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{5B2F0353-95F8-4DCF-B3BC-0BBE000EB8F6}" uniqueName="3" name="At_Situacao" queryTableFieldId="3" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{E7CE68CB-A1FF-46BC-93BE-9116EBA50B9F}" uniqueName="4" name="At_DataRef" queryTableFieldId="4" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{5C9C4225-6BE7-4955-A793-8C860651F33E}" uniqueName="5" name="At_DataInicio" queryTableFieldId="5" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{893E6C04-AFB9-4B12-A199-D4BE6562C55D}" uniqueName="6" name="At_DataFim" queryTableFieldId="6" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{05DB2C07-4238-48EB-9DF6-4A14F78EB259}" uniqueName="7" name="At_ValidadeDias" queryTableFieldId="7" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{32D990E8-9596-4F1C-801B-85A44CDE7A5D}" uniqueName="8" name="At_DtFimValidade" queryTableFieldId="8" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{02AAD34D-9B73-4D07-A0E3-444E8706BC37}" name="ProcessosAtualizacao" displayName="ProcessosAtualizacao" ref="A1:I5" tableType="queryTable" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{02AAD34D-9B73-4D07-A0E3-444E8706BC37}" name="ProcessosAtualizacao" displayName="ProcessosAtualizacao" ref="A1:I5" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:I5" xr:uid="{02AAD34D-9B73-4D07-A0E3-444E8706BC37}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{980C5C42-9BA4-493C-AA04-A61ECBD61636}" uniqueName="1" name="ControleAt_Id" queryTableFieldId="1" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{94731E6A-DEB2-4CE2-B3CE-0D6A8653A50B}" uniqueName="2" name="At_id" queryTableFieldId="2" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4D7ABFE7-11E1-4910-838B-F176115AC818}" uniqueName="3" name="Data" queryTableFieldId="3" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{1602AE87-05F5-41BB-B265-80E66906119F}" uniqueName="4" name="Processo_id" queryTableFieldId="4" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{4FD02EC4-2164-4CD8-BE7A-643F7A9BD1CC}" uniqueName="5" name="Processo_Nome" queryTableFieldId="5" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{68692FAD-45AA-4ECB-A9DD-56526EFCE049}" uniqueName="6" name="Completo" queryTableFieldId="6" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{C521AFA8-268C-405A-9C24-C6B789846D2D}" uniqueName="7" name="DataInicio" queryTableFieldId="7" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{1231BACB-CED4-47B7-B5B8-198DCA61F730}" uniqueName="8" name="DataFim" queryTableFieldId="8" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{02A80D39-D3CC-4622-A140-1DA5395E8456}" uniqueName="9" name="Controle" queryTableFieldId="9" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{980C5C42-9BA4-493C-AA04-A61ECBD61636}" uniqueName="1" name="ControleAt_Id" queryTableFieldId="1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{94731E6A-DEB2-4CE2-B3CE-0D6A8653A50B}" uniqueName="2" name="At_id" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{4D7ABFE7-11E1-4910-838B-F176115AC818}" uniqueName="3" name="Data" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{1602AE87-05F5-41BB-B265-80E66906119F}" uniqueName="4" name="Processo_id" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{4FD02EC4-2164-4CD8-BE7A-643F7A9BD1CC}" uniqueName="5" name="Processo_Nome" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{68692FAD-45AA-4ECB-A9DD-56526EFCE049}" uniqueName="6" name="Completo" queryTableFieldId="6" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{C521AFA8-268C-405A-9C24-C6B789846D2D}" uniqueName="7" name="DataInicio" queryTableFieldId="7" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{1231BACB-CED4-47B7-B5B8-198DCA61F730}" uniqueName="8" name="DataFim" queryTableFieldId="8" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{02A80D39-D3CC-4622-A140-1DA5395E8456}" uniqueName="9" name="Controle" queryTableFieldId="9" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6F985DA8-6DB5-4A78-927C-52ADCD70BD3C}" name="BackupsFiles" displayName="BackupsFiles" ref="A1:D4" tableType="queryTable" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6F985DA8-6DB5-4A78-927C-52ADCD70BD3C}" name="BackupsFiles" displayName="BackupsFiles" ref="A1:D4" tableType="queryTable" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:D4" xr:uid="{6F985DA8-6DB5-4A78-927C-52ADCD70BD3C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{89F68E51-D022-4971-85A2-D612525ED1AF}" uniqueName="1" name="ControleAt_Id" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C1DB6770-A6B0-4272-82C5-8CCBC7C9731C}" uniqueName="2" name="FileFolder" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{06CC5E6E-2A8E-4E7D-A39D-2714A210F739}" uniqueName="3" name="FileName" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{69CE5A60-7849-4093-98A6-ED3B039BE50C}" uniqueName="4" name="FileSizeMB" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{89F68E51-D022-4971-85A2-D612525ED1AF}" uniqueName="1" name="ControleAt_Id" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C1DB6770-A6B0-4272-82C5-8CCBC7C9731C}" uniqueName="2" name="FileFolder" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{06CC5E6E-2A8E-4E7D-A39D-2714A210F739}" uniqueName="3" name="FileName" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{69CE5A60-7849-4093-98A6-ED3B039BE50C}" uniqueName="4" name="FileSizeMB" queryTableFieldId="4" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427F3ED8-1754-4C90-A0D4-A386BBEA70A5}" name="tb_Processos" displayName="tb_Processos" ref="A1:D8" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A1:D8" xr:uid="{427F3ED8-1754-4C90-A0D4-A386BBEA70A5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D7">
-    <sortCondition ref="C1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{427F3ED8-1754-4C90-A0D4-A386BBEA70A5}" name="tb_Processos" displayName="tb_Processos" ref="A1:D10" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:D10" xr:uid="{427F3ED8-1754-4C90-A0D4-A386BBEA70A5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
+    <sortCondition ref="C1:C9"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9622D56B-CC45-4B19-AF22-CD56603C2150}" name="id" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{9622D56B-CC45-4B19-AF22-CD56603C2150}" name="id" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{6599EC34-2FD9-4F38-A5A1-BEE2A4D1BFDA}" name="Processo"/>
     <tableColumn id="3" xr3:uid="{D5A79581-48FF-42AD-90B3-C59179E93B03}" name="Ordem" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{331886DB-6E42-4E32-92B8-40599C2FC1FA}" name="Dt_UltimaExecucao" dataDxfId="0">
@@ -502,9 +503,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -542,7 +543,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -648,7 +649,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -790,7 +791,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -804,19 +805,19 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -842,14 +843,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="5">
@@ -858,7 +859,7 @@
       <c r="E2" s="5">
         <v>45238.333333333336</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="2">
@@ -884,19 +885,19 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -925,8 +926,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="2">
@@ -938,7 +939,7 @@
       <c r="D2" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="2">
@@ -954,8 +955,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2">
@@ -967,7 +968,7 @@
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="2">
@@ -983,8 +984,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2">
@@ -996,7 +997,7 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="2">
@@ -1012,8 +1013,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="2">
@@ -1025,7 +1026,7 @@
       <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="2">
@@ -1057,15 +1058,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1075,43 +1076,43 @@
       <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>95.155104492187505</v>
       </c>
     </row>
@@ -1132,14 +1133,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1163,21 +1164,21 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FA919B-3014-4FD1-B7FF-96A96DC11F44}">
   <sheetPr codeName="Planilha5"/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>5</v>
       </c>
@@ -1206,7 +1207,7 @@
         <v>45240.364982175925</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>45238.333333333336</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>45240.304861111108</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1251,12 +1252,12 @@
         <v>45254.537645219905</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -1266,11 +1267,14 @@
         <v>.</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="str">
@@ -1278,14 +1282,47 @@
         <v>.</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" s="3" t="str">
+        <f>IF(COUNTIF(ProcessosAtualizacao[Processo_id],tb_Processos[[#This Row],[id]])=0,".",_xlfn.MAXIFS(ProcessosAtualizacao[DataFim],ProcessosAtualizacao[Processo_id],tb_Processos[[#This Row],[id]]))</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>IF(COUNTIF(ProcessosAtualizacao[Processo_id],tb_Processos[[#This Row],[id]])=0,".",_xlfn.MAXIFS(ProcessosAtualizacao[DataFim],ProcessosAtualizacao[Processo_id],tb_Processos[[#This Row],[id]]))</f>
+        <v>.</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="3" t="str">
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="str">
         <f>IF(COUNTIF(ProcessosAtualizacao[Processo_id],tb_Processos[[#This Row],[id]])=0,".",_xlfn.MAXIFS(ProcessosAtualizacao[DataFim],ProcessosAtualizacao[Processo_id],tb_Processos[[#This Row],[id]]))</f>
         <v>.</v>
       </c>

</xml_diff>